<commit_message>
Added unique username check
</commit_message>
<xml_diff>
--- a/testdata/users.xlsx
+++ b/testdata/users.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>FirstName</t>
   </si>
@@ -59,40 +59,34 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>FName1gg</t>
-  </si>
-  <si>
-    <t>LName1gg</t>
-  </si>
-  <si>
-    <t>User1gg</t>
-  </si>
-  <si>
-    <t>admin@mail.comgg</t>
-  </si>
-  <si>
-    <t>082555gg</t>
-  </si>
-  <si>
-    <t>Pass1gg</t>
-  </si>
-  <si>
-    <t>Pass1hh</t>
-  </si>
-  <si>
-    <t>083444hh</t>
-  </si>
-  <si>
-    <t>cusomter@mail.comhh</t>
-  </si>
-  <si>
-    <t>User2hh</t>
-  </si>
-  <si>
-    <t>LName2hh</t>
-  </si>
-  <si>
-    <t>FName2hh</t>
+    <t>admin@mail.com</t>
+  </si>
+  <si>
+    <t>cusomter@mail.com</t>
+  </si>
+  <si>
+    <t>FName1yy</t>
+  </si>
+  <si>
+    <t>LName1yy</t>
+  </si>
+  <si>
+    <t>User#1yy</t>
+  </si>
+  <si>
+    <t>082555yy</t>
+  </si>
+  <si>
+    <t>Pass1yy</t>
+  </si>
+  <si>
+    <t>083444yy</t>
+  </si>
+  <si>
+    <t>LName2yy</t>
+  </si>
+  <si>
+    <t>FName2yy</t>
   </si>
 </sst>
 </file>
@@ -425,7 +419,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,25 +462,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
@@ -494,19 +488,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>18</v>

</xml_diff>